<commit_message>
final version for submission
</commit_message>
<xml_diff>
--- a/data/ECB_projections.xlsx
+++ b/data/ECB_projections.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\macrometrics-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\macrometrics-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC0F1C2-DBB1-4754-B906-E38C826B78F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3648822F-5B7B-49E2-BA7C-5D08CB1F159D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{12C7916D-DF84-4674-81AC-F6E6A0DFF915}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -419,11 +419,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C816B2E1-F2BF-400D-A7E0-BDA34F77B681}">
-  <dimension ref="B2:D118"/>
+  <dimension ref="B2:D110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -444,29 +442,29 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
-        <v>35885</v>
+        <v>36616</v>
       </c>
       <c r="C3" s="4">
-        <v>0.7</v>
+        <v>1.2</v>
       </c>
       <c r="D3" s="4">
-        <v>0.7</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
-        <v>35976</v>
+        <v>36707</v>
       </c>
       <c r="C4" s="4">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D4" s="4">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
-        <v>36068</v>
+        <v>36799</v>
       </c>
       <c r="C5" s="4">
         <v>0.6</v>
@@ -477,18 +475,18 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
-        <v>36160</v>
+        <v>36891</v>
       </c>
       <c r="C6" s="4">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="D6" s="4">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
-        <v>36250</v>
+        <v>36981</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -499,95 +497,95 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
-        <v>36341</v>
+        <v>37072</v>
       </c>
       <c r="C8" s="4">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="D8" s="4">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
-        <v>36433</v>
+        <v>37164</v>
       </c>
       <c r="C9" s="4">
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
       <c r="D9" s="4">
-        <v>1.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
-        <v>36525</v>
+        <v>37256</v>
       </c>
       <c r="C10" s="4">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="D10" s="4">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
-        <v>36616</v>
+        <v>37346</v>
       </c>
       <c r="C11" s="4">
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
       <c r="D11" s="4">
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
-        <v>36707</v>
+        <v>37437</v>
       </c>
       <c r="C12" s="4">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="D12" s="4">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
-        <v>36799</v>
+        <v>37529</v>
       </c>
       <c r="C13" s="4">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D13" s="4">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
-        <v>36891</v>
+        <v>37621</v>
       </c>
       <c r="C14" s="4">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="D14" s="4">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="1">
-        <v>36981</v>
+        <v>37711</v>
       </c>
       <c r="C15" s="4">
-        <v>1</v>
+        <v>-0.3</v>
       </c>
       <c r="D15" s="4">
-        <v>1</v>
+        <v>-0.3</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
-        <v>37072</v>
+        <v>37802</v>
       </c>
       <c r="C16" s="4">
         <v>0.1</v>
@@ -598,271 +596,271 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="1">
-        <v>37164</v>
+        <v>37894</v>
       </c>
       <c r="C17" s="4">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="D17" s="4">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="1">
-        <v>37256</v>
+        <v>37986</v>
       </c>
       <c r="C18" s="4">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="D18" s="4">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="1">
-        <v>37346</v>
+        <v>38077</v>
       </c>
       <c r="C19" s="4">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D19" s="4">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
-        <v>37437</v>
+        <v>38168</v>
       </c>
       <c r="C20" s="4">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D20" s="4">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="1">
-        <v>37529</v>
+        <v>38260</v>
       </c>
       <c r="C21" s="4">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D21" s="4">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="1">
-        <v>37621</v>
+        <v>38352</v>
       </c>
       <c r="C22" s="4">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D22" s="4">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="1">
-        <v>37711</v>
+        <v>38442</v>
       </c>
       <c r="C23" s="4">
-        <v>-0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D23" s="4">
-        <v>-0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="1">
-        <v>37802</v>
+        <v>38533</v>
       </c>
       <c r="C24" s="4">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="D24" s="4">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="1">
-        <v>37894</v>
+        <v>38625</v>
       </c>
       <c r="C25" s="4">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D25" s="4">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="1">
-        <v>37986</v>
+        <v>38717</v>
       </c>
       <c r="C26" s="4">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="D26" s="4">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="1">
-        <v>38077</v>
+        <v>38807</v>
       </c>
       <c r="C27" s="4">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D27" s="4">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" s="1">
-        <v>38168</v>
+        <v>38898</v>
       </c>
       <c r="C28" s="4">
-        <v>0.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D28" s="4">
-        <v>0.6</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="1">
-        <v>38260</v>
+        <v>38990</v>
       </c>
       <c r="C29" s="4">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="D29" s="4">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="1">
-        <v>38352</v>
+        <v>39082</v>
       </c>
       <c r="C30" s="4">
-        <v>0.4</v>
+        <v>1.2</v>
       </c>
       <c r="D30" s="4">
-        <v>0.4</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="1">
-        <v>38442</v>
+        <v>39172</v>
       </c>
       <c r="C31" s="4">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="D31" s="4">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" s="1">
-        <v>38533</v>
+        <v>39263</v>
       </c>
       <c r="C32" s="4">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="D32" s="4">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" s="1">
-        <v>38625</v>
+        <v>39355</v>
       </c>
       <c r="C33" s="4">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D33" s="4">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="1">
-        <v>38717</v>
+        <v>39447</v>
       </c>
       <c r="C34" s="4">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="D34" s="4">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" s="1">
-        <v>38807</v>
+        <v>39538</v>
       </c>
       <c r="C35" s="4">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D35" s="4">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" s="1">
-        <v>38898</v>
+        <v>39629</v>
       </c>
       <c r="C36" s="4">
-        <v>1.1000000000000001</v>
+        <v>-0.4</v>
       </c>
       <c r="D36" s="4">
-        <v>1.1000000000000001</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B37" s="1">
-        <v>38990</v>
+        <v>39721</v>
       </c>
       <c r="C37" s="4">
-        <v>0.6</v>
+        <v>-0.5</v>
       </c>
       <c r="D37" s="4">
-        <v>0.6</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="1">
-        <v>39082</v>
+        <v>39813</v>
       </c>
       <c r="C38" s="4">
-        <v>1.2</v>
+        <v>-1.8</v>
       </c>
       <c r="D38" s="4">
-        <v>1.2</v>
+        <v>-1.8</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B39" s="1">
-        <v>39172</v>
+        <v>39903</v>
       </c>
       <c r="C39" s="4">
-        <v>0.6</v>
+        <v>-3.1</v>
       </c>
       <c r="D39" s="4">
-        <v>0.6</v>
+        <v>-3.1</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B40" s="1">
-        <v>39263</v>
+        <v>39994</v>
       </c>
       <c r="C40" s="4">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="D40" s="4">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B41" s="1">
-        <v>39355</v>
+        <v>40086</v>
       </c>
       <c r="C41" s="4">
         <v>0.4</v>
@@ -873,7 +871,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B42" s="1">
-        <v>39447</v>
+        <v>40178</v>
       </c>
       <c r="C42" s="4">
         <v>0.5</v>
@@ -884,62 +882,62 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B43" s="1">
-        <v>39538</v>
+        <v>40268</v>
       </c>
       <c r="C43" s="4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D43" s="4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B44" s="1">
-        <v>39629</v>
+        <v>40359</v>
       </c>
       <c r="C44" s="4">
-        <v>-0.4</v>
+        <v>1</v>
       </c>
       <c r="D44" s="4">
-        <v>-0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B45" s="1">
-        <v>39721</v>
+        <v>40451</v>
       </c>
       <c r="C45" s="4">
-        <v>-0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D45" s="4">
-        <v>-0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B46" s="1">
-        <v>39813</v>
+        <v>40543</v>
       </c>
       <c r="C46" s="4">
-        <v>-1.8</v>
+        <v>0.6</v>
       </c>
       <c r="D46" s="4">
-        <v>-1.8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B47" s="1">
-        <v>39903</v>
+        <v>40633</v>
       </c>
       <c r="C47" s="4">
-        <v>-3.1</v>
+        <v>0.9</v>
       </c>
       <c r="D47" s="4">
-        <v>-3.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B48" s="1">
-        <v>39994</v>
+        <v>40724</v>
       </c>
       <c r="C48" s="4">
         <v>0</v>
@@ -950,216 +948,216 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B49" s="1">
-        <v>40086</v>
+        <v>40816</v>
       </c>
       <c r="C49" s="4">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="D49" s="4">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B50" s="1">
-        <v>40178</v>
+        <v>40908</v>
       </c>
       <c r="C50" s="4">
-        <v>0.5</v>
+        <v>-0.4</v>
       </c>
       <c r="D50" s="4">
-        <v>0.5</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B51" s="1">
-        <v>40268</v>
+        <v>40999</v>
       </c>
       <c r="C51" s="4">
-        <v>0.4</v>
+        <v>-0.2</v>
       </c>
       <c r="D51" s="4">
-        <v>0.4</v>
+        <v>-0.3</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B52" s="1">
-        <v>40359</v>
+        <v>41090</v>
       </c>
       <c r="C52" s="4">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="D52" s="4">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B53" s="1">
-        <v>40451</v>
+        <v>41182</v>
       </c>
       <c r="C53" s="4">
-        <v>0.4</v>
+        <v>-0.1</v>
       </c>
       <c r="D53" s="4">
-        <v>0.4</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B54" s="1">
-        <v>40543</v>
+        <v>41274</v>
       </c>
       <c r="C54" s="4">
-        <v>0.6</v>
+        <v>-0.5</v>
       </c>
       <c r="D54" s="4">
-        <v>0.6</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B55" s="1">
-        <v>40633</v>
+        <v>41364</v>
       </c>
       <c r="C55" s="4">
-        <v>0.9</v>
+        <v>-0.4</v>
       </c>
       <c r="D55" s="4">
-        <v>0.9</v>
+        <v>-0.3</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B56" s="1">
-        <v>40724</v>
+        <v>41455</v>
       </c>
       <c r="C56" s="4">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D56" s="4">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B57" s="1">
-        <v>40816</v>
+        <v>41547</v>
       </c>
       <c r="C57" s="4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D57" s="4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B58" s="1">
-        <v>40908</v>
+        <v>41639</v>
       </c>
       <c r="C58" s="4">
-        <v>-0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D58" s="4">
-        <v>-0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B59" s="1">
-        <v>40999</v>
+        <v>41729</v>
       </c>
       <c r="C59" s="4">
-        <v>-0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D59" s="4">
-        <v>-0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B60" s="1">
-        <v>41090</v>
+        <v>41820</v>
       </c>
       <c r="C60" s="4">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="D60" s="4">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B61" s="1">
-        <v>41182</v>
+        <v>41912</v>
       </c>
       <c r="C61" s="4">
-        <v>-0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D61" s="4">
-        <v>-0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B62" s="1">
-        <v>41274</v>
+        <v>42004</v>
       </c>
       <c r="C62" s="4">
-        <v>-0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D62" s="4">
-        <v>-0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B63" s="1">
-        <v>41364</v>
+        <v>42094</v>
       </c>
       <c r="C63" s="4">
-        <v>-0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D63" s="4">
-        <v>-0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B64" s="1">
-        <v>41455</v>
+        <v>42185</v>
       </c>
       <c r="C64" s="4">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="D64" s="4">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B65" s="1">
-        <v>41547</v>
+        <v>42277</v>
       </c>
       <c r="C65" s="4">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D65" s="4">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B66" s="1">
-        <v>41639</v>
+        <v>42369</v>
       </c>
       <c r="C66" s="4">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D66" s="4">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B67" s="1">
-        <v>41729</v>
+        <v>42460</v>
       </c>
       <c r="C67" s="4">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D67" s="4">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B68" s="1">
-        <v>41820</v>
+        <v>42551</v>
       </c>
       <c r="C68" s="4">
         <v>0.2</v>
@@ -1170,7 +1168,7 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B69" s="1">
-        <v>41912</v>
+        <v>42643</v>
       </c>
       <c r="C69" s="4">
         <v>0.5</v>
@@ -1181,351 +1179,351 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B70" s="1">
-        <v>42004</v>
+        <v>42735</v>
       </c>
       <c r="C70" s="4">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D70" s="4">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B71" s="1">
-        <v>42094</v>
+        <v>42825</v>
       </c>
       <c r="C71" s="4">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="D71" s="4">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B72" s="1">
-        <v>42185</v>
+        <v>42916</v>
       </c>
       <c r="C72" s="4">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D72" s="4">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B73" s="1">
-        <v>42277</v>
+        <v>43008</v>
       </c>
       <c r="C73" s="4">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="D73" s="4">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B74" s="1">
-        <v>42369</v>
+        <v>43100</v>
       </c>
       <c r="C74" s="4">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D74" s="4">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B75" s="1">
-        <v>42460</v>
+        <v>43190</v>
       </c>
       <c r="C75" s="4">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="D75" s="4">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B76" s="1">
-        <v>42551</v>
+        <v>43281</v>
       </c>
       <c r="C76" s="4">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="D76" s="4">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B77" s="1">
-        <v>42643</v>
+        <v>43373</v>
       </c>
       <c r="C77" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D77" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B78" s="1">
-        <v>42735</v>
+        <v>43465</v>
       </c>
       <c r="C78" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="D78" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B79" s="1">
-        <v>42825</v>
+        <v>43555</v>
       </c>
       <c r="C79" s="4">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="D79" s="4">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B80" s="1">
-        <v>42916</v>
+        <v>43646</v>
       </c>
       <c r="C80" s="4">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D80" s="4">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B81" s="1">
-        <v>43008</v>
+        <v>43738</v>
       </c>
       <c r="C81" s="4">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="D81" s="4">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B82" s="1">
-        <v>43100</v>
+        <v>43830</v>
       </c>
       <c r="C82" s="4">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="D82" s="4">
-        <v>0.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B83" s="1">
-        <v>43190</v>
+        <v>43921</v>
       </c>
       <c r="C83" s="4">
-        <v>0</v>
+        <v>-3.4</v>
       </c>
       <c r="D83" s="4">
-        <v>0</v>
+        <v>-3.4</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B84" s="1">
-        <v>43281</v>
+        <v>44012</v>
       </c>
       <c r="C84" s="4">
-        <v>0.6</v>
+        <v>-11.3</v>
       </c>
       <c r="D84" s="4">
-        <v>0.6</v>
+        <v>-11.3</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B85" s="1">
-        <v>43373</v>
+        <v>44104</v>
       </c>
       <c r="C85" s="4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D85" s="4">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B86" s="1">
-        <v>43465</v>
+        <v>44196</v>
       </c>
       <c r="C86" s="4">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="D86" s="4">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B87" s="1">
-        <v>43555</v>
+        <v>44286</v>
       </c>
       <c r="C87" s="4">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="D87" s="4">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B88" s="1">
-        <v>43646</v>
+        <v>44377</v>
       </c>
       <c r="C88" s="4">
-        <v>0.4</v>
+        <v>2.1</v>
       </c>
       <c r="D88" s="4">
-        <v>0.4</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B89" s="1">
-        <v>43738</v>
+        <v>44469</v>
       </c>
       <c r="C89" s="4">
-        <v>0.2</v>
+        <v>2.1</v>
       </c>
       <c r="D89" s="4">
-        <v>0.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B90" s="1">
-        <v>43830</v>
+        <v>44561</v>
       </c>
       <c r="C90" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D90" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B91" s="1">
-        <v>43921</v>
+        <v>44651</v>
       </c>
       <c r="C91" s="4">
-        <v>-3.4</v>
+        <v>0.7</v>
       </c>
       <c r="D91" s="4">
-        <v>-3.4</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B92" s="1">
-        <v>44012</v>
+        <v>44742</v>
       </c>
       <c r="C92" s="4">
-        <v>-11.3</v>
+        <v>0.8</v>
       </c>
       <c r="D92" s="4">
-        <v>-11.3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B93" s="1">
-        <v>44104</v>
+        <v>44834</v>
       </c>
       <c r="C93" s="4">
-        <v>12</v>
+        <v>0.5</v>
       </c>
       <c r="D93" s="4">
-        <v>12</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B94" s="1">
-        <v>44196</v>
+        <v>44926</v>
       </c>
       <c r="C94" s="4">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="D94" s="4">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B95" s="1">
-        <v>44286</v>
+        <v>45016</v>
       </c>
       <c r="C95" s="4">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="D95" s="4">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B96" s="1">
-        <v>44377</v>
+        <v>45107</v>
       </c>
       <c r="C96" s="4">
-        <v>2.1</v>
+        <v>0.1</v>
       </c>
       <c r="D96" s="4">
-        <v>2.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B97" s="1">
-        <v>44469</v>
+        <v>45199</v>
       </c>
       <c r="C97" s="4">
-        <v>2.1</v>
+        <v>0</v>
       </c>
       <c r="D97" s="4">
-        <v>2</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B98" s="1">
-        <v>44561</v>
+        <v>45291</v>
       </c>
       <c r="C98" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D98" s="4">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B99" s="1">
-        <v>44651</v>
+        <v>45382</v>
       </c>
       <c r="C99" s="4">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="D99" s="4">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B100" s="1">
-        <v>44742</v>
+        <v>45473</v>
       </c>
       <c r="C100" s="4">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="D100" s="4">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B101" s="1">
-        <v>44834</v>
+        <v>45565</v>
       </c>
       <c r="C101" s="4">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D101" s="4">
         <v>0.4</v>
@@ -1533,87 +1531,87 @@
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B102" s="1">
-        <v>44926</v>
+        <v>45657</v>
       </c>
       <c r="C102" s="4">
-        <v>-0.1</v>
+        <v>0.4</v>
       </c>
       <c r="D102" s="4">
-        <v>-0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B103" s="1">
-        <v>45016</v>
+        <v>45747</v>
       </c>
       <c r="C103" s="4">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="D103" s="4">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B104" s="1">
-        <v>45107</v>
+        <v>45838</v>
       </c>
       <c r="C104" s="4">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="D104" s="4">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B105" s="1">
-        <v>45199</v>
+        <v>45930</v>
       </c>
       <c r="C105" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D105" s="4">
-        <v>-0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B106" s="1">
-        <v>45291</v>
+        <v>46022</v>
       </c>
       <c r="C106" s="4">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D106" s="4">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B107" s="1">
-        <v>45382</v>
+        <v>46112</v>
       </c>
       <c r="C107" s="4">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="D107" s="4">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B108" s="1">
-        <v>45473</v>
+        <v>46203</v>
       </c>
       <c r="C108" s="4">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D108" s="4">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B109" s="1">
-        <v>45565</v>
+        <v>46295</v>
       </c>
       <c r="C109" s="4">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D109" s="4">
         <v>0.4</v>
@@ -1621,100 +1619,12 @@
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B110" s="1">
-        <v>45657</v>
+        <v>46387</v>
       </c>
       <c r="C110" s="4">
         <v>0.4</v>
       </c>
       <c r="D110" s="4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B111" s="1">
-        <v>45747</v>
-      </c>
-      <c r="C111" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D111" s="4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B112" s="1">
-        <v>45838</v>
-      </c>
-      <c r="C112" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D112" s="4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B113" s="1">
-        <v>45930</v>
-      </c>
-      <c r="C113" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D113" s="4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B114" s="1">
-        <v>46022</v>
-      </c>
-      <c r="C114" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D114" s="4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B115" s="1">
-        <v>46112</v>
-      </c>
-      <c r="C115" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D115" s="4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B116" s="1">
-        <v>46203</v>
-      </c>
-      <c r="C116" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D116" s="4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B117" s="1">
-        <v>46295</v>
-      </c>
-      <c r="C117" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D117" s="4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B118" s="1">
-        <v>46387</v>
-      </c>
-      <c r="C118" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D118" s="4">
         <v>0.4</v>
       </c>
     </row>

</xml_diff>